<commit_message>
Updated myRIO Demo Board to Rev 1.1. Modified component IDs for manufacturing. Adjusted silk screen.
</commit_message>
<xml_diff>
--- a/myRIO/Demo Board/myRIODemoBoard_BOM.xlsx
+++ b/myRIO/Demo Board/myRIODemoBoard_BOM.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
   <si>
     <t>Manufacturer</t>
   </si>
@@ -90,12 +90,6 @@
     <t>CONN FMALE 34POS DL .1" R/A GOLD</t>
   </si>
   <si>
-    <t>Through Hole, Right Angle</t>
-  </si>
-  <si>
-    <t>myRIO MXP</t>
-  </si>
-  <si>
     <t>C1</t>
   </si>
   <si>
@@ -138,9 +132,6 @@
     <t>Through Hole</t>
   </si>
   <si>
-    <t>7SEG1</t>
-  </si>
-  <si>
     <t>160-2013-5-ND</t>
   </si>
   <si>
@@ -150,10 +141,16 @@
     <t>DISPLAY 1DGT GREEN 0.56" CA</t>
   </si>
   <si>
-    <t>10-DIP (0.600", 15.24mm)</t>
-  </si>
-  <si>
     <t>Header</t>
+  </si>
+  <si>
+    <t>10-DIP</t>
+  </si>
+  <si>
+    <t>SEV_SEG1</t>
+  </si>
+  <si>
+    <t>MXP1</t>
   </si>
 </sst>
 </file>
@@ -598,7 +595,7 @@
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -661,7 +658,7 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="D3" t="s">
         <v>1</v>
@@ -676,10 +673,10 @@
         <v>23</v>
       </c>
       <c r="H3" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="I3" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -690,7 +687,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D4" t="s">
         <v>4</v>
@@ -699,16 +696,16 @@
         <v>5</v>
       </c>
       <c r="F4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" t="s">
         <v>27</v>
       </c>
-      <c r="G4" t="s">
-        <v>28</v>
-      </c>
-      <c r="H4" t="s">
-        <v>29</v>
-      </c>
       <c r="I4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -719,7 +716,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D5" t="s">
         <v>6</v>
@@ -728,16 +725,16 @@
         <v>7</v>
       </c>
       <c r="F5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H5" t="s">
         <v>31</v>
       </c>
-      <c r="H5" t="s">
-        <v>33</v>
-      </c>
       <c r="I5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -748,22 +745,22 @@
         <v>1</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G6" t="s">
         <v>35</v>
       </c>
-      <c r="E6" t="s">
-        <v>36</v>
-      </c>
-      <c r="F6" t="s">
-        <v>34</v>
-      </c>
-      <c r="G6" t="s">
+      <c r="I6" t="s">
         <v>37</v>
-      </c>
-      <c r="I6" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -774,25 +771,25 @@
         <v>1</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="D7" t="s">
         <v>3</v>
       </c>
       <c r="E7" t="s">
+        <v>39</v>
+      </c>
+      <c r="F7" t="s">
+        <v>38</v>
+      </c>
+      <c r="G7" t="s">
+        <v>40</v>
+      </c>
+      <c r="H7" t="s">
         <v>42</v>
       </c>
-      <c r="F7" t="s">
-        <v>41</v>
-      </c>
-      <c r="G7" t="s">
-        <v>43</v>
-      </c>
-      <c r="H7" t="s">
-        <v>44</v>
-      </c>
       <c r="I7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:9">

</xml_diff>

<commit_message>
Updated BOM and component IDs to work better with Screaming Circuits  parser
</commit_message>
<xml_diff>
--- a/myRIO/Demo Board/myRIODemoBoard_BOM.xlsx
+++ b/myRIO/Demo Board/myRIODemoBoard_BOM.xlsx
@@ -147,10 +147,10 @@
     <t>10-DIP</t>
   </si>
   <si>
-    <t>SEV_SEG1</t>
-  </si>
-  <si>
     <t>MXP1</t>
+  </si>
+  <si>
+    <t>SEG1</t>
   </si>
 </sst>
 </file>
@@ -595,7 +595,7 @@
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -658,7 +658,7 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D3" t="s">
         <v>1</v>
@@ -771,7 +771,7 @@
         <v>1</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D7" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
Updated R1 to 200k in schematic, BOM and silkscreen Generated new gerbers.
</commit_message>
<xml_diff>
--- a/myRIO/Demo Board/myRIODemoBoard_BOM.xlsx
+++ b/myRIO/Demo Board/myRIODemoBoard_BOM.xlsx
@@ -39,9 +39,6 @@
     <t>Stackpole Electronics Inc</t>
   </si>
   <si>
-    <t>CF14JT1K00</t>
-  </si>
-  <si>
     <t>Item #</t>
   </si>
   <si>
@@ -102,12 +99,6 @@
     <t>Radial, Can</t>
   </si>
   <si>
-    <t>CF14JT1K00CT-ND</t>
-  </si>
-  <si>
-    <t>RES 1K OHM 1/4W 5% CARBON FILM</t>
-  </si>
-  <si>
     <t>R1</t>
   </si>
   <si>
@@ -151,6 +142,15 @@
   </si>
   <si>
     <t>SEG1</t>
+  </si>
+  <si>
+    <t>CF14JT200K</t>
+  </si>
+  <si>
+    <t>CF14JT200KCT-ND</t>
+  </si>
+  <si>
+    <t>RES 200K OHM 1/4W 5% CARBON FILM</t>
   </si>
 </sst>
 </file>
@@ -263,7 +263,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -298,6 +298,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -595,7 +600,7 @@
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -613,31 +618,31 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -658,7 +663,7 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D3" t="s">
         <v>1</v>
@@ -667,16 +672,16 @@
         <v>2</v>
       </c>
       <c r="F3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" t="s">
         <v>22</v>
       </c>
-      <c r="G3" t="s">
-        <v>23</v>
-      </c>
       <c r="H3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="I3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -687,7 +692,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D4" t="s">
         <v>4</v>
@@ -696,45 +701,45 @@
         <v>5</v>
       </c>
       <c r="F4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" t="s">
         <v>25</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>26</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="14">
+        <v>3</v>
+      </c>
+      <c r="B5" s="14">
+        <v>1</v>
+      </c>
+      <c r="C5" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="I4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" s="4">
-        <v>3</v>
-      </c>
-      <c r="B5" s="4">
-        <v>1</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="D5" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="E5" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" t="s">
+      <c r="E5" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="F5" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="G5" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="H5" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="G5" t="s">
-        <v>29</v>
-      </c>
-      <c r="H5" t="s">
-        <v>31</v>
-      </c>
-      <c r="I5" t="s">
-        <v>37</v>
+      <c r="I5" s="16" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -745,22 +750,22 @@
         <v>1</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D6" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" t="s">
+        <v>32</v>
+      </c>
+      <c r="I6" t="s">
         <v>34</v>
-      </c>
-      <c r="F6" t="s">
-        <v>32</v>
-      </c>
-      <c r="G6" t="s">
-        <v>35</v>
-      </c>
-      <c r="I6" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -771,25 +776,25 @@
         <v>1</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D7" t="s">
         <v>3</v>
       </c>
       <c r="E7" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" t="s">
+        <v>35</v>
+      </c>
+      <c r="G7" t="s">
+        <v>37</v>
+      </c>
+      <c r="H7" t="s">
         <v>39</v>
       </c>
-      <c r="F7" t="s">
-        <v>38</v>
-      </c>
-      <c r="G7" t="s">
-        <v>40</v>
-      </c>
-      <c r="H7" t="s">
-        <v>42</v>
-      </c>
       <c r="I7" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -807,14 +812,14 @@
     <row r="10" spans="1:9">
       <c r="B10" s="4"/>
       <c r="G10" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H10" s="13"/>
     </row>
     <row r="11" spans="1:9">
       <c r="B11" s="4"/>
       <c r="G11" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H11" s="9">
         <v>5</v>
@@ -823,7 +828,7 @@
     <row r="12" spans="1:9">
       <c r="B12" s="4"/>
       <c r="G12" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H12" s="9">
         <v>0</v>
@@ -832,7 +837,7 @@
     <row r="13" spans="1:9">
       <c r="B13" s="4"/>
       <c r="G13" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H13" s="9">
         <v>5</v>
@@ -841,7 +846,7 @@
     <row r="14" spans="1:9">
       <c r="B14" s="4"/>
       <c r="G14" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H14" s="9">
         <f>SUMIF($I$8:$I$16, "fine pitch", $B$8:$B$16)</f>
@@ -851,7 +856,7 @@
     <row r="15" spans="1:9" ht="15.75" thickBot="1">
       <c r="B15" s="4"/>
       <c r="G15" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H15" s="11">
         <f>SUMIF($I$8:$I$16, "bga", $B$8:$B$16)</f>

</xml_diff>